<commit_message>
update meet up entry
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myngu\Desktop\GIT\Frogger_to_the_max\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786F3D1A-53F9-4B46-8E72-50C89B4236DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C5377F-EF10-4999-B779-AB4977AF176B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{1DAC1EE6-F3C8-4CA5-B6DA-A9CA82F18626}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="49">
   <si>
     <t>Tasks</t>
   </si>
@@ -66,9 +66,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>Undecided</t>
-  </si>
-  <si>
     <t xml:space="preserve">Design </t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Create the font (.png) (32x32 pixels)</t>
   </si>
   <si>
-    <t>Timer</t>
-  </si>
-  <si>
     <t>Background (Top and Bottom)</t>
   </si>
   <si>
@@ -175,6 +169,15 @@
   </si>
   <si>
     <t>We agreed that we going to meet up 3:30  every Tuesday until the project is due</t>
+  </si>
+  <si>
+    <t>My</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Everyone</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +242,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -252,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -293,6 +302,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E58E5856-C891-4BF8-B0A4-C56ADB4EBC85}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:L6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +636,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -642,7 +654,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -723,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
@@ -752,234 +764,267 @@
         <v>10</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="D9" s="15"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>15</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>16</v>
       </c>
       <c r="D10" s="16"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D11" s="14"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>18</v>
-      </c>
-      <c r="C12" s="15" t="s">
-        <v>19</v>
       </c>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>20</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>21</v>
       </c>
       <c r="E13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="E14" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>24</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>25</v>
       </c>
       <c r="D16" s="17"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="11"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="E19" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+        <v>28</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+        <v>47</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+        <v>32</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J27" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="12"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="K28" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L28" s="12"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="K29" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="L29" s="12"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="L32" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="D17:E17"/>
+  <mergeCells count="24">
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="E19:I19"/>
+    <mergeCell ref="E24:I24"/>
+    <mergeCell ref="E25:I25"/>
+    <mergeCell ref="E21:I21"/>
+    <mergeCell ref="E22:I22"/>
+    <mergeCell ref="E20:I20"/>
+    <mergeCell ref="E23:I23"/>
+    <mergeCell ref="C17:D17"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:N2"/>
     <mergeCell ref="C6:L6"/>

</xml_diff>